<commit_message>
Update project structure and add logging for DataFrames.  Cast column types.
</commit_message>
<xml_diff>
--- a/data/clean/Juniors_2024.xlsx
+++ b/data/clean/Juniors_2024.xlsx
@@ -1168,11 +1168,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="A10" s="11" t="n"/>
       <c r="B10" s="11" t="inlineStr">
         <is>
           <t>Johnson Dillon</t>
@@ -4516,11 +4512,7 @@
       <c r="AD22" s="25" t="n"/>
     </row>
     <row r="23" ht="13.5" customHeight="1" s="45">
-      <c r="A23" s="23" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="A23" s="23" t="n"/>
       <c r="B23" s="23" t="inlineStr">
         <is>
           <t>Virta Akseli</t>
@@ -9182,11 +9174,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="11" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="A42" s="11" t="n"/>
       <c r="B42" s="11" t="inlineStr">
         <is>
           <t>Mok Julian</t>

</xml_diff>